<commit_message>
looked at optics documentation+start(example) code
</commit_message>
<xml_diff>
--- a/Sprint2/week4/Group25 DBL Scrum Timesheets.xlsx
+++ b/Sprint2/week4/Group25 DBL Scrum Timesheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G\Documents\Documenten TU-Eindhoven\Year 1 - Q4\DBL C++\Github\Embedded_system_group25\Sprint2\week4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/c_i_zanders_student_tue_nl/Documents/Documents/gitkraken/Embedded_system_group25/Sprint2/week4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527FD3A7-780A-46D2-9306-262FD32D9861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{527FD3A7-780A-46D2-9306-262FD32D9861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{579D0021-7879-4ABB-8DA2-7F431515BD5B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -1076,7 +1076,7 @@
                   <c:v>1.2506944444444443</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.39583333333333337</c:v>
+                  <c:v>0.95833333333333337</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.70833333333333326</c:v>
@@ -1174,7 +1174,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2091029163"/>
@@ -1250,7 +1250,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="443840806"/>
@@ -1273,7 +1273,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1314,7 +1314,7 @@
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.7298611111111108</c:v>
+                  <c:v>1.9381944444444443</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.3645833333333333</c:v>
@@ -1323,10 +1323,10 @@
                   <c:v>1.3229166666666665</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4791666666666667</c:v>
+                  <c:v>1.6041666666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.22916666666666666</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1353,7 +1353,7 @@
                 <c:formatCode>[h]:mm</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.7298611111111108</c:v>
+                  <c:v>1.9381944444444443</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.3645833333333333</c:v>
@@ -1362,10 +1362,10 @@
                   <c:v>1.3229166666666665</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4791666666666667</c:v>
+                  <c:v>1.6041666666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.22916666666666666</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1446,7 +1446,7 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1669176459"/>
@@ -1492,7 +1492,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1911,7 +1911,7 @@
                   <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8333333333333333</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2002,7 +2002,7 @@
               <a:latin typeface="+mn-lt"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4218,7 +4218,7 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -16528,7 +16528,7 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
@@ -24650,8 +24650,8 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24855,15 +24855,21 @@
         <f t="array" ref="B10">INDEX(Tasks,5,2)</f>
         <v>Lectures/Plenary meetings</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="14">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="D10" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E10" s="44">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
+      <c r="F10" s="44">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G10" s="44">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="H10" s="44"/>
       <c r="I10" s="11"/>
       <c r="J10" s="44"/>
@@ -24885,15 +24891,21 @@
         <f t="array" ref="B11">INDEX(Tasks,6,2)</f>
         <v>Sprint Tasks</v>
       </c>
-      <c r="C11" s="10"/>
+      <c r="C11" s="14">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D11" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E11" s="44">
         <v>0.14583333333333334</v>
       </c>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="F11" s="44">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G11" s="44">
+        <v>6.25E-2</v>
+      </c>
       <c r="H11" s="39"/>
       <c r="I11" s="44"/>
       <c r="J11" s="39"/>
@@ -24915,7 +24927,9 @@
         <f t="array" ref="B12">INDEX(Tasks,7,2)</f>
         <v xml:space="preserve">Sprint Task 1.1: Read course material </v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="11">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D12" s="11"/>
       <c r="E12" s="44"/>
       <c r="F12" s="44"/>
@@ -27665,7 +27679,7 @@
       </c>
       <c r="C128" s="46">
         <f t="shared" ref="C128:L128" si="0">SUM(C5:C127)</f>
-        <v>0</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="D128" s="46">
         <f t="shared" si="0"/>
@@ -27677,11 +27691,11 @@
       </c>
       <c r="F128" s="46">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="G128" s="46">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="H128" s="46">
         <f t="shared" si="0"/>
@@ -27734,43 +27748,43 @@
       </c>
       <c r="C130" s="12">
         <f>SUM(C128)</f>
-        <v>0</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="D130" s="39">
         <f>SUM(D128,C128)</f>
-        <v>0.16666666666666666</v>
+        <v>0.375</v>
       </c>
       <c r="E130" s="39">
         <f>SUM(E128,C128,D128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="F130" s="39">
         <f>SUM(C128:F128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.72916666666666674</v>
       </c>
       <c r="G130" s="39">
         <f>SUM(C128:G128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="H130" s="39">
         <f>SUM(C128:H128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="I130" s="39">
         <f>SUM(C128:I128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="J130" s="39">
         <f>SUM(C128:J128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="K130" s="39">
         <f>SUM(C128:K128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="L130" s="39">
         <f>SUM(C128:L128)</f>
-        <v>0.39583333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="M130" s="47"/>
       <c r="O130" s="39"/>
@@ -27790,43 +27804,43 @@
       </c>
       <c r="C131" s="39">
         <f>Parameters!$G$9-C130</f>
-        <v>5.833333333333333</v>
+        <v>5.625</v>
       </c>
       <c r="D131" s="39">
         <f>Parameters!$G$9-D130</f>
-        <v>5.6666666666666661</v>
+        <v>5.458333333333333</v>
       </c>
       <c r="E131" s="39">
         <f>Parameters!$G$9-E130</f>
-        <v>5.4375</v>
+        <v>5.2291666666666661</v>
       </c>
       <c r="F131" s="39">
         <f>Parameters!$G$9-F130</f>
-        <v>5.4375</v>
+        <v>5.1041666666666661</v>
       </c>
       <c r="G131" s="39">
         <f>Parameters!$G$9-G130</f>
-        <v>5.4375</v>
+        <v>4.875</v>
       </c>
       <c r="H131" s="39">
         <f>Parameters!$G$9-H130</f>
-        <v>5.4375</v>
+        <v>4.875</v>
       </c>
       <c r="I131" s="39">
         <f>Parameters!$G$9-I130</f>
-        <v>5.4375</v>
+        <v>4.875</v>
       </c>
       <c r="J131" s="39">
         <f>Parameters!$G$9-J130</f>
-        <v>5.4375</v>
+        <v>4.875</v>
       </c>
       <c r="K131" s="39">
         <f>Parameters!$G$9-K130</f>
-        <v>5.4375</v>
+        <v>4.875</v>
       </c>
       <c r="L131" s="39">
         <f>Parameters!$G$9-L130</f>
-        <v>5.4375</v>
+        <v>4.875</v>
       </c>
       <c r="O131" s="39"/>
       <c r="P131" s="39"/>
@@ -28728,7 +28742,7 @@
   </sheetPr>
   <dimension ref="B1:N1062"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B140" sqref="B140"/>
     </sheetView>
   </sheetViews>
@@ -29009,7 +29023,7 @@
       </c>
       <c r="C10" s="48">
         <f>SUM('Serkan Efe Durusu'!C10,'Ismail Elmasry'!C10,'can Işmar'!C10,'Marios Papalouka'!C10,'Metehan Topaç'!C10,'Celine Zanders '!C10)</f>
-        <v>0.72916666666666663</v>
+        <v>0.89583333333333326</v>
       </c>
       <c r="D10" s="48">
         <f>SUM('Serkan Efe Durusu'!D10,'Ismail Elmasry'!D10,'can Işmar'!D10,'Marios Papalouka'!D10,'Metehan Topaç'!D10,'Celine Zanders '!D10)</f>
@@ -29021,11 +29035,11 @@
       </c>
       <c r="F10" s="48">
         <f>SUM('Serkan Efe Durusu'!F10,'Ismail Elmasry'!F10,'can Işmar'!F10,'Marios Papalouka'!F10,'Metehan Topaç'!F10,'Celine Zanders '!F10)</f>
-        <v>0.25</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G10" s="48">
         <f>SUM('Serkan Efe Durusu'!G10,'Ismail Elmasry'!G10,'can Işmar'!G10,'Marios Papalouka'!G10,'Metehan Topaç'!G10,'Celine Zanders '!G10)</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H10" s="48">
         <f>SUM('Serkan Efe Durusu'!H10,'Ismail Elmasry'!H10,'can Işmar'!H10,'Marios Papalouka'!H10,'Metehan Topaç'!H10,'Celine Zanders '!H10)</f>
@@ -29049,7 +29063,7 @@
       </c>
       <c r="M10" s="51">
         <f t="shared" si="0"/>
-        <v>1.8333333333333333</v>
+        <v>2.25</v>
       </c>
       <c r="N10" s="50" t="str">
         <f t="array" ref="N10">IF(INDEX(Tasks,1,3)&lt;&gt;"",100*M10/INDEX(Tasks,1,3),"")</f>
@@ -29063,7 +29077,7 @@
       </c>
       <c r="C11" s="48">
         <f>SUM('Serkan Efe Durusu'!C11,'Ismail Elmasry'!C11,'can Işmar'!C11,'Marios Papalouka'!C11,'Metehan Topaç'!D11,'Celine Zanders '!C11)</f>
-        <v>0.39583333333333331</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="D11" s="48" t="e">
         <f>SUM('Serkan Efe Durusu'!D11,'Ismail Elmasry'!D11,'can Işmar'!D11,'Marios Papalouka'!D11,'Metehan Topaç'!#REF!,'Celine Zanders '!D11)</f>
@@ -29075,11 +29089,11 @@
       </c>
       <c r="F11" s="48">
         <f>SUM('Serkan Efe Durusu'!F11,'Ismail Elmasry'!F11,'can Işmar'!F11,'Marios Papalouka'!F11,'Metehan Topaç'!F11,'Celine Zanders '!F11)</f>
-        <v>0.625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G11" s="48">
         <f>SUM('Serkan Efe Durusu'!G11,'Ismail Elmasry'!G11,'can Işmar'!G11,'Marios Papalouka'!G11,'Metehan Topaç'!G11,'Celine Zanders '!G11)</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H11" s="48">
         <f>SUM('Serkan Efe Durusu'!H11,'Ismail Elmasry'!H11,'can Işmar'!H11,'Marios Papalouka'!H11,'Metehan Topaç'!H11,'Celine Zanders '!H11)</f>
@@ -29117,7 +29131,7 @@
       </c>
       <c r="C12" s="48">
         <f>SUM('Serkan Efe Durusu'!C12,'Ismail Elmasry'!C12,'can Işmar'!C12,'Marios Papalouka'!C12,'Metehan Topaç'!D12,'Celine Zanders '!C12)</f>
-        <v>0.22916666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="D12" s="48" t="e">
         <f>SUM('Serkan Efe Durusu'!D12,'Ismail Elmasry'!D12,'can Işmar'!D12,'Marios Papalouka'!D12,'Metehan Topaç'!#REF!,'Celine Zanders '!D12)</f>
@@ -35208,7 +35222,7 @@
       </c>
       <c r="C136" s="26">
         <f>'Celine Zanders '!C128</f>
-        <v>0</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="D136" s="26">
         <f>'Celine Zanders '!D128</f>
@@ -35220,11 +35234,11 @@
       </c>
       <c r="F136" s="26">
         <f>'Celine Zanders '!F128</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="G136" s="26">
         <f>'Celine Zanders '!G128</f>
-        <v>0</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="H136" s="26">
         <f>'Celine Zanders '!H128</f>
@@ -35248,7 +35262,7 @@
       </c>
       <c r="M136" s="54">
         <f t="shared" si="1"/>
-        <v>0.39583333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
     </row>
     <row r="137" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -35534,7 +35548,7 @@
     <row r="143" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C143" s="54">
         <f t="shared" ref="C143:L143" si="2">SUM(C135:C142)</f>
-        <v>1.7298611111111108</v>
+        <v>1.9381944444444443</v>
       </c>
       <c r="D143" s="54">
         <f t="shared" si="2"/>
@@ -35546,11 +35560,11 @@
       </c>
       <c r="F143" s="54">
         <f t="shared" si="2"/>
-        <v>1.4791666666666667</v>
+        <v>1.6041666666666667</v>
       </c>
       <c r="G143" s="54">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="H143" s="54">
         <f t="shared" si="2"/>
@@ -35574,7 +35588,7 @@
       </c>
       <c r="M143" s="54">
         <f t="shared" si="1"/>
-        <v>5.896527777777778</v>
+        <v>6.459027777777778</v>
       </c>
     </row>
     <row r="144" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>